<commit_message>
Putting Things Together 1
Massive changes to the structure.
- Added lots of Interface Classes along with Implementation Classes
</commit_message>
<xml_diff>
--- a/data/staff_list.xlsx
+++ b/data/staff_list.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\LF work\LF running courses\CX2002\Assignment\2023S1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive - Nanyang Technological University\Y2S1\SC2002\CampManagement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD0A763-F36A-4773-B526-842599E71A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A8423552-B407-44FC-A4E0-CF93C2750A9A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
+    <workbookView windowHeight="11295" windowWidth="21600" xWindow="4605" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}" yWindow="2460"/>
   </bookViews>
   <sheets>
-    <sheet name="staff" sheetId="1" r:id="rId1"/>
+    <sheet name="staff" r:id="rId1" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$B$88</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
+    <definedName localSheetId="0" name="_xlnm.Print_Area">staff!$A$1:$B$88</definedName>
+    <definedName localSheetId="0" name="_xlnm.Print_Titles">staff!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Datta</t>
   </si>
   <si>
-    <t xml:space="preserve">Arvind </t>
-  </si>
-  <si>
     <t>ARVI@NTU.EDU.SG</t>
   </si>
   <si>
@@ -89,13 +86,35 @@
   </si>
   <si>
     <t>HUKUMAR@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Arvind</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +176,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -180,31 +207,32 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="13">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -221,10 +249,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -259,7 +287,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -311,7 +339,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -422,21 +450,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -453,7 +481,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -505,29 +533,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:C87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
+      <selection activeCell="E6" pane="bottomLeft" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="7" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="7" width="22.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -537,377 +565,413 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="2"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="2"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="2"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="6"/>
       <c r="B36" s="3"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="2"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="2"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="2"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="3"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="2"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="2"/>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="2"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="2"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="2"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="2"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="2"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="3"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="2"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="2"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="2"/>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="2"/>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="2"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="2"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="2"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="2"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="2"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="10"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="2"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="2"/>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="2"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="2"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="2"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="2"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="2"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="2"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{81D093B7-7D45-4C94-BB5C-7AACAE95581C}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{9931FE22-2FDA-4031-AC32-E8C581BFEA0B}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{C6203F7B-B631-4F6A-ABDC-A4C27A0A1DAD}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{49DFE096-5F31-4004-8F65-766F1044AD00}"/>
-    <hyperlink ref="B2" r:id="rId5" xr:uid="{0B389DC2-D438-4218-8936-76A694EA9F12}"/>
+    <hyperlink r:id="rId1" ref="B6" xr:uid="{81D093B7-7D45-4C94-BB5C-7AACAE95581C}"/>
+    <hyperlink r:id="rId2" ref="B5" xr:uid="{9931FE22-2FDA-4031-AC32-E8C581BFEA0B}"/>
+    <hyperlink r:id="rId3" ref="B4" xr:uid="{C6203F7B-B631-4F6A-ABDC-A4C27A0A1DAD}"/>
+    <hyperlink r:id="rId4" ref="B3" xr:uid="{49DFE096-5F31-4004-8F65-766F1044AD00}"/>
+    <hyperlink r:id="rId5" ref="B2" xr:uid="{0B389DC2-D438-4218-8936-76A694EA9F12}"/>
   </hyperlinks>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageMargins bottom="0.74803149606299213" footer="0.31496062992125984" header="0.31496062992125984" left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed Saving role and committeeOf outside
- Only persistent data saved outside is password now
</commit_message>
<xml_diff>
--- a/data/staff_list.xlsx
+++ b/data/staff_list.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\OneDrive - Nanyang Technological University\Y2S1\SC2002\CampManagement\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A8423552-B407-44FC-A4E0-CF93C2750A9A}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF0CDE6-CCFA-4B4F-A687-9E81DE5F46C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="11295" windowWidth="21600" xWindow="4605" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}" yWindow="2460"/>
+    <workbookView xWindow="4605" yWindow="2460" windowWidth="21600" windowHeight="11295" xr2:uid="{A1AB1725-9614-4760-9E35-FCE78E076BF2}"/>
   </bookViews>
   <sheets>
-    <sheet name="staff" r:id="rId1" sheetId="1"/>
+    <sheet name="staff" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName localSheetId="0" name="_xlnm.Print_Area">staff!$A$1:$B$88</definedName>
-    <definedName localSheetId="0" name="_xlnm.Print_Titles">staff!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">staff!$A$1:$B$88</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">staff!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -94,16 +94,7 @@
     <t>password</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
-    <t>Staff</t>
-  </si>
-  <si>
     <t>Arvind</t>
-  </si>
-  <si>
-    <t>123</t>
   </si>
   <si>
     <t>1</t>
@@ -113,7 +104,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,32 +197,32 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="9" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="3" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="6" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="8" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="4" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="9" numFmtId="49" xfId="1"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -249,10 +239,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -287,7 +277,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -339,7 +329,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -450,21 +440,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -481,7 +471,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -533,26 +523,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
-  <dimension ref="A1:F87"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55DE67C8-F00F-4E71-A7B2-83068F640C77}">
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection activeCell="E6" pane="bottomLeft" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="7" width="22.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.5703125" collapsed="true"/>
+    <col min="1" max="1" width="22" style="7" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -568,9 +558,7 @@
       <c r="D1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="E1" s="12"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -585,9 +573,6 @@
       <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -602,9 +587,6 @@
       <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -619,9 +601,6 @@
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -636,13 +615,10 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>11</v>
@@ -651,9 +627,6 @@
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -965,13 +938,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B6" xr:uid="{81D093B7-7D45-4C94-BB5C-7AACAE95581C}"/>
-    <hyperlink r:id="rId2" ref="B5" xr:uid="{9931FE22-2FDA-4031-AC32-E8C581BFEA0B}"/>
-    <hyperlink r:id="rId3" ref="B4" xr:uid="{C6203F7B-B631-4F6A-ABDC-A4C27A0A1DAD}"/>
-    <hyperlink r:id="rId4" ref="B3" xr:uid="{49DFE096-5F31-4004-8F65-766F1044AD00}"/>
-    <hyperlink r:id="rId5" ref="B2" xr:uid="{0B389DC2-D438-4218-8936-76A694EA9F12}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{81D093B7-7D45-4C94-BB5C-7AACAE95581C}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{9931FE22-2FDA-4031-AC32-E8C581BFEA0B}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{C6203F7B-B631-4F6A-ABDC-A4C27A0A1DAD}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{49DFE096-5F31-4004-8F65-766F1044AD00}"/>
+    <hyperlink ref="B2" r:id="rId5" xr:uid="{0B389DC2-D438-4218-8936-76A694EA9F12}"/>
   </hyperlinks>
-  <pageMargins bottom="0.74803149606299213" footer="0.31496062992125984" header="0.31496062992125984" left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId6"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>